<commit_message>
30th May 25 - Practice
</commit_message>
<xml_diff>
--- a/TestData/DataHomePage1.xlsx
+++ b/TestData/DataHomePage1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanky Verma\OneDrive\Desktop\Python Selenium\WorkSpace2\1stFebPythonSelenium_Framework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanky Verma\PycharmProjects\PythonProject\PythonProject\Framework_Demo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Sr No.</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Product  Price($)</t>
+  </si>
+  <si>
+    <t>Swag Labs</t>
+  </si>
+  <si>
+    <t>Title=</t>
   </si>
 </sst>
 </file>
@@ -137,8 +143,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Sr No." dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="2" name="Product Name " dataDxfId="3" totalsRowDxfId="2"/>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,6 +518,15 @@
         <v>129.94</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
31th May 25 - updated
</commit_message>
<xml_diff>
--- a/TestData/DataHomePage1.xlsx
+++ b/TestData/DataHomePage1.xlsx
@@ -56,10 +56,10 @@
     <t>Product  Price($)</t>
   </si>
   <si>
+    <t>Title=</t>
+  </si>
+  <si>
     <t>Swag Labs</t>
-  </si>
-  <si>
-    <t>Title=</t>
   </si>
 </sst>
 </file>
@@ -520,10 +520,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C9" s="1"/>
     </row>

</xml_diff>

<commit_message>
1st June 25 - updated
</commit_message>
<xml_diff>
--- a/TestData/DataHomePage1.xlsx
+++ b/TestData/DataHomePage1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Sr No.</t>
   </si>
@@ -50,13 +50,16 @@
     <t>Test.allTheThings() T-Shirt (Red)</t>
   </si>
   <si>
-    <t>Total =</t>
-  </si>
-  <si>
     <t>Product  Price($)</t>
   </si>
   <si>
     <t>Swag Labs</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Total=</t>
   </si>
 </sst>
 </file>
@@ -92,19 +95,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -143,12 +149,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:C9"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Sr No." dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="Product Name " dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="3" name="Product  Price($)" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:D8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sr No." dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Product Name " dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Product  Price($)" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Column1" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -425,12 +432,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,10 +446,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -451,8 +462,11 @@
       <c r="C2" s="1">
         <v>29.99</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -462,8 +476,9 @@
       <c r="C3" s="1">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -473,8 +488,9 @@
       <c r="C4" s="1">
         <v>15.99</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -484,8 +500,9 @@
       <c r="C5" s="1">
         <v>49.99</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -495,8 +512,9 @@
       <c r="C6" s="1">
         <v>7.99</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -506,10 +524,11 @@
       <c r="C7" s="1">
         <v>15.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>6</v>
@@ -517,13 +536,7 @@
       <c r="C8" s="1">
         <v>129.94</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>